<commit_message>
Last Commit on 5May2023
</commit_message>
<xml_diff>
--- a/OtherDocs/TestcaseFile/AMS_TestCase_File.xlsx
+++ b/OtherDocs/TestcaseFile/AMS_TestCase_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\Selenabler_Framework\Selenabler2.0\OtherDocs\TestcaseFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E9EF56-D838-4235-AF4E-01B41F006EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930CBCAA-E37A-4976-96B7-BA04A33C6C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" xr2:uid="{B641B8B7-5EE6-4DB7-B527-98A5312C13C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="773" activeTab="1" xr2:uid="{B641B8B7-5EE6-4DB7-B527-98A5312C13C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Profile" sheetId="8" r:id="rId1"/>
@@ -6173,6 +6173,35 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6200,9 +6229,6 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6220,6 +6246,53 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6300,54 +6373,6 @@
     <xf numFmtId="0" fontId="14" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -6377,6 +6402,48 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6414,13 +6481,7 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6459,71 +6520,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="53" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8040,8 +8040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710B5436-AE10-4376-92F6-DE75C0736E51}">
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8051,51 +8051,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B2" s="243"/>
+      <c r="B2" s="136"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" thickTop="1">
-      <c r="B3" s="244"/>
-      <c r="C3" s="240" t="s">
+      <c r="B3" s="158"/>
+      <c r="C3" s="152" t="s">
         <v>501</v>
       </c>
-      <c r="D3" s="136"/>
+      <c r="D3" s="153"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="245"/>
-      <c r="C4" s="241"/>
-      <c r="D4" s="238"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="154"/>
+      <c r="D4" s="155"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B5" s="246"/>
-      <c r="C5" s="242"/>
-      <c r="D5" s="239"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="157"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="43" t="s">
         <v>492</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="140" t="s">
         <v>468</v>
       </c>
-      <c r="D6" s="131"/>
+      <c r="D6" s="141"/>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="36" t="s">
         <v>493</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="142" t="s">
         <v>501</v>
       </c>
-      <c r="D7" s="133"/>
+      <c r="D7" s="143"/>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="36" t="s">
         <v>494</v>
       </c>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="144" t="s">
         <v>549</v>
       </c>
-      <c r="D8" s="135"/>
+      <c r="D8" s="145"/>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1">
       <c r="B9" s="44" t="s">
@@ -8107,16 +8107,16 @@
       <c r="D9" s="45"/>
     </row>
     <row r="10" spans="2:4" ht="13.5" customHeight="1">
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="146" t="s">
         <v>671</v>
       </c>
-      <c r="C10" s="138"/>
-      <c r="D10" s="139"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="148"/>
     </row>
     <row r="11" spans="2:4" ht="0.75" customHeight="1" thickBot="1">
-      <c r="B11" s="140"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="142"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="151"/>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="46" t="s">
@@ -8205,19 +8205,19 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B20" s="127"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="129"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="138"/>
+      <c r="D20" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="B3:B5"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B10:D11"/>
-    <mergeCell ref="C3:D5"/>
-    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D19" location="RTM!C2" display="go_to_RTM_url" xr:uid="{0553300D-95EC-4C18-9727-B1D163850DE1}"/>
@@ -8332,13 +8332,13 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="30">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="240" t="s">
         <v>532</v>
       </c>
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="204" t="s">
         <v>829</v>
       </c>
-      <c r="C2" s="217" t="s">
+      <c r="C2" s="237" t="s">
         <v>849</v>
       </c>
       <c r="D2" s="92" t="s">
@@ -8397,9 +8397,9 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="48" customHeight="1">
-      <c r="A3" s="221"/>
-      <c r="B3" s="222"/>
-      <c r="C3" s="218"/>
+      <c r="A3" s="241"/>
+      <c r="B3" s="242"/>
+      <c r="C3" s="238"/>
       <c r="D3" s="92" t="s">
         <v>481</v>
       </c>
@@ -8456,9 +8456,9 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="51" customHeight="1">
-      <c r="A4" s="221"/>
-      <c r="B4" s="222"/>
-      <c r="C4" s="218"/>
+      <c r="A4" s="241"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="238"/>
       <c r="D4" s="92" t="s">
         <v>481</v>
       </c>
@@ -8515,9 +8515,9 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="33" customHeight="1">
-      <c r="A5" s="221"/>
-      <c r="B5" s="222"/>
-      <c r="C5" s="219"/>
+      <c r="A5" s="241"/>
+      <c r="B5" s="242"/>
+      <c r="C5" s="239"/>
       <c r="D5" s="92" t="s">
         <v>481</v>
       </c>
@@ -8574,9 +8574,9 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="48" customHeight="1">
-      <c r="A6" s="221"/>
-      <c r="B6" s="222"/>
-      <c r="C6" s="217" t="s">
+      <c r="A6" s="241"/>
+      <c r="B6" s="242"/>
+      <c r="C6" s="237" t="s">
         <v>857</v>
       </c>
       <c r="D6" s="92" t="s">
@@ -8635,9 +8635,9 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="48" customHeight="1">
-      <c r="A7" s="221"/>
-      <c r="B7" s="222"/>
-      <c r="C7" s="218"/>
+      <c r="A7" s="241"/>
+      <c r="B7" s="242"/>
+      <c r="C7" s="238"/>
       <c r="D7" s="92" t="s">
         <v>481</v>
       </c>
@@ -8694,9 +8694,9 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="30.75" customHeight="1">
-      <c r="A8" s="221"/>
-      <c r="B8" s="222"/>
-      <c r="C8" s="218"/>
+      <c r="A8" s="241"/>
+      <c r="B8" s="242"/>
+      <c r="C8" s="238"/>
       <c r="D8" s="92" t="s">
         <v>481</v>
       </c>
@@ -8753,9 +8753,9 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="36" customHeight="1">
-      <c r="A9" s="221"/>
-      <c r="B9" s="222"/>
-      <c r="C9" s="218"/>
+      <c r="A9" s="241"/>
+      <c r="B9" s="242"/>
+      <c r="C9" s="238"/>
       <c r="D9" s="92" t="s">
         <v>481</v>
       </c>
@@ -8810,9 +8810,9 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="34.5" customHeight="1">
-      <c r="A10" s="221"/>
-      <c r="B10" s="222"/>
-      <c r="C10" s="218"/>
+      <c r="A10" s="241"/>
+      <c r="B10" s="242"/>
+      <c r="C10" s="238"/>
       <c r="D10" s="92" t="s">
         <v>481</v>
       </c>
@@ -8869,9 +8869,9 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="25.5" customHeight="1">
-      <c r="A11" s="221"/>
-      <c r="B11" s="222"/>
-      <c r="C11" s="218"/>
+      <c r="A11" s="241"/>
+      <c r="B11" s="242"/>
+      <c r="C11" s="238"/>
       <c r="D11" s="92" t="s">
         <v>481</v>
       </c>
@@ -8928,9 +8928,9 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="33" customHeight="1">
-      <c r="A12" s="221"/>
-      <c r="B12" s="222"/>
-      <c r="C12" s="219"/>
+      <c r="A12" s="241"/>
+      <c r="B12" s="242"/>
+      <c r="C12" s="239"/>
       <c r="D12" s="92" t="s">
         <v>481</v>
       </c>
@@ -8987,9 +8987,9 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="34.5" customHeight="1">
-      <c r="A13" s="221"/>
-      <c r="B13" s="222"/>
-      <c r="C13" s="217" t="s">
+      <c r="A13" s="241"/>
+      <c r="B13" s="242"/>
+      <c r="C13" s="237" t="s">
         <v>865</v>
       </c>
       <c r="D13" s="92" t="s">
@@ -9048,9 +9048,9 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45" customHeight="1">
-      <c r="A14" s="221"/>
-      <c r="B14" s="222"/>
-      <c r="C14" s="218"/>
+      <c r="A14" s="241"/>
+      <c r="B14" s="242"/>
+      <c r="C14" s="238"/>
       <c r="D14" s="92" t="s">
         <v>481</v>
       </c>
@@ -9107,9 +9107,9 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="33" customHeight="1">
-      <c r="A15" s="221"/>
-      <c r="B15" s="222"/>
-      <c r="C15" s="218"/>
+      <c r="A15" s="241"/>
+      <c r="B15" s="242"/>
+      <c r="C15" s="238"/>
       <c r="D15" s="92" t="s">
         <v>481</v>
       </c>
@@ -9166,9 +9166,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="37.5" customHeight="1">
-      <c r="A16" s="221"/>
-      <c r="B16" s="222"/>
-      <c r="C16" s="218"/>
+      <c r="A16" s="241"/>
+      <c r="B16" s="242"/>
+      <c r="C16" s="238"/>
       <c r="D16" s="92" t="s">
         <v>481</v>
       </c>
@@ -9221,9 +9221,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="33" customHeight="1">
-      <c r="A17" s="221"/>
-      <c r="B17" s="222"/>
-      <c r="C17" s="218"/>
+      <c r="A17" s="241"/>
+      <c r="B17" s="242"/>
+      <c r="C17" s="238"/>
       <c r="D17" s="92" t="s">
         <v>481</v>
       </c>
@@ -9280,9 +9280,9 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="36.75" customHeight="1">
-      <c r="A18" s="221"/>
-      <c r="B18" s="222"/>
-      <c r="C18" s="218"/>
+      <c r="A18" s="241"/>
+      <c r="B18" s="242"/>
+      <c r="C18" s="238"/>
       <c r="D18" s="92" t="s">
         <v>481</v>
       </c>
@@ -9339,9 +9339,9 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="36.75" customHeight="1">
-      <c r="A19" s="221"/>
-      <c r="B19" s="222"/>
-      <c r="C19" s="219"/>
+      <c r="A19" s="241"/>
+      <c r="B19" s="242"/>
+      <c r="C19" s="239"/>
       <c r="D19" s="92" t="s">
         <v>481</v>
       </c>
@@ -9398,9 +9398,9 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="37.5" customHeight="1">
-      <c r="A20" s="221"/>
-      <c r="B20" s="222"/>
-      <c r="C20" s="217" t="s">
+      <c r="A20" s="241"/>
+      <c r="B20" s="242"/>
+      <c r="C20" s="237" t="s">
         <v>899</v>
       </c>
       <c r="D20" s="92" t="s">
@@ -9459,9 +9459,9 @@
       </c>
     </row>
     <row r="21" spans="1:23" ht="30.75" customHeight="1">
-      <c r="A21" s="221"/>
-      <c r="B21" s="197"/>
-      <c r="C21" s="219"/>
+      <c r="A21" s="241"/>
+      <c r="B21" s="205"/>
+      <c r="C21" s="239"/>
       <c r="D21" s="92" t="s">
         <v>481</v>
       </c>
@@ -9684,10 +9684,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="233" t="s">
         <v>533</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="206" t="s">
         <v>589</v>
       </c>
       <c r="C2" s="26" t="s">
@@ -9749,8 +9749,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="60.75" customHeight="1">
-      <c r="A3" s="214"/>
-      <c r="B3" s="186"/>
+      <c r="A3" s="234"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="23" t="s">
         <v>590</v>
       </c>
@@ -9810,8 +9810,8 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="24" customHeight="1">
-      <c r="A4" s="214"/>
-      <c r="B4" s="186"/>
+      <c r="A4" s="234"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="21" t="s">
         <v>487</v>
       </c>
@@ -9871,9 +9871,9 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="25.5" customHeight="1">
-      <c r="A5" s="214"/>
-      <c r="B5" s="186"/>
-      <c r="C5" s="176" t="s">
+      <c r="A5" s="234"/>
+      <c r="B5" s="207"/>
+      <c r="C5" s="209" t="s">
         <v>593</v>
       </c>
       <c r="D5" s="26" t="s">
@@ -9932,9 +9932,9 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="27.75" customHeight="1">
-      <c r="A6" s="214"/>
-      <c r="B6" s="186"/>
-      <c r="C6" s="178"/>
+      <c r="A6" s="234"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="211"/>
       <c r="D6" s="26" t="s">
         <v>481</v>
       </c>
@@ -9991,9 +9991,9 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="27.75" customHeight="1">
-      <c r="A7" s="214"/>
-      <c r="B7" s="186"/>
-      <c r="C7" s="176" t="s">
+      <c r="A7" s="234"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="209" t="s">
         <v>594</v>
       </c>
       <c r="D7" s="26" t="s">
@@ -10052,9 +10052,9 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="27.75" customHeight="1">
-      <c r="A8" s="214"/>
-      <c r="B8" s="186"/>
-      <c r="C8" s="177"/>
+      <c r="A8" s="234"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="210"/>
       <c r="D8" s="26" t="s">
         <v>481</v>
       </c>
@@ -10111,9 +10111,9 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="24" customHeight="1">
-      <c r="A9" s="214"/>
-      <c r="B9" s="186"/>
-      <c r="C9" s="177"/>
+      <c r="A9" s="234"/>
+      <c r="B9" s="207"/>
+      <c r="C9" s="210"/>
       <c r="D9" s="26" t="s">
         <v>481</v>
       </c>
@@ -10170,9 +10170,9 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="25.5" customHeight="1">
-      <c r="A10" s="214"/>
-      <c r="B10" s="186"/>
-      <c r="C10" s="177"/>
+      <c r="A10" s="234"/>
+      <c r="B10" s="207"/>
+      <c r="C10" s="210"/>
       <c r="D10" s="26" t="s">
         <v>481</v>
       </c>
@@ -10229,9 +10229,9 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="24.75" customHeight="1">
-      <c r="A11" s="214"/>
-      <c r="B11" s="186"/>
-      <c r="C11" s="177"/>
+      <c r="A11" s="234"/>
+      <c r="B11" s="207"/>
+      <c r="C11" s="210"/>
       <c r="D11" s="26" t="s">
         <v>481</v>
       </c>
@@ -10288,9 +10288,9 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="24" customHeight="1">
-      <c r="A12" s="214"/>
-      <c r="B12" s="186"/>
-      <c r="C12" s="178"/>
+      <c r="A12" s="234"/>
+      <c r="B12" s="207"/>
+      <c r="C12" s="211"/>
       <c r="D12" s="26" t="s">
         <v>481</v>
       </c>
@@ -10347,8 +10347,8 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="24.75" customHeight="1">
-      <c r="A13" s="214"/>
-      <c r="B13" s="186"/>
+      <c r="A13" s="234"/>
+      <c r="B13" s="207"/>
       <c r="C13" s="26" t="s">
         <v>593</v>
       </c>
@@ -10408,8 +10408,8 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="35.25" customHeight="1">
-      <c r="A14" s="214"/>
-      <c r="B14" s="186"/>
+      <c r="A14" s="234"/>
+      <c r="B14" s="207"/>
       <c r="C14" s="23" t="s">
         <v>596</v>
       </c>
@@ -10463,8 +10463,8 @@
       <c r="W14" s="9"/>
     </row>
     <row r="15" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A15" s="214"/>
-      <c r="B15" s="186"/>
+      <c r="A15" s="234"/>
+      <c r="B15" s="207"/>
       <c r="C15" s="26" t="s">
         <v>597</v>
       </c>
@@ -10518,8 +10518,8 @@
       <c r="W15" s="9"/>
     </row>
     <row r="16" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A16" s="214"/>
-      <c r="B16" s="186"/>
+      <c r="A16" s="234"/>
+      <c r="B16" s="207"/>
       <c r="C16" s="26" t="s">
         <v>595</v>
       </c>
@@ -10573,9 +10573,9 @@
       <c r="W16" s="9"/>
     </row>
     <row r="17" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A17" s="214"/>
-      <c r="B17" s="186"/>
-      <c r="C17" s="176" t="s">
+      <c r="A17" s="234"/>
+      <c r="B17" s="207"/>
+      <c r="C17" s="209" t="s">
         <v>597</v>
       </c>
       <c r="D17" s="26" t="s">
@@ -10628,9 +10628,9 @@
       <c r="W17" s="9"/>
     </row>
     <row r="18" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A18" s="214"/>
-      <c r="B18" s="186"/>
-      <c r="C18" s="178"/>
+      <c r="A18" s="234"/>
+      <c r="B18" s="207"/>
+      <c r="C18" s="211"/>
       <c r="D18" s="26" t="s">
         <v>481</v>
       </c>
@@ -10681,9 +10681,9 @@
       <c r="W18" s="9"/>
     </row>
     <row r="19" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A19" s="214"/>
-      <c r="B19" s="186"/>
-      <c r="C19" s="176" t="s">
+      <c r="A19" s="234"/>
+      <c r="B19" s="207"/>
+      <c r="C19" s="209" t="s">
         <v>595</v>
       </c>
       <c r="D19" s="26" t="s">
@@ -10736,9 +10736,9 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A20" s="214"/>
-      <c r="B20" s="186"/>
-      <c r="C20" s="177"/>
+      <c r="A20" s="234"/>
+      <c r="B20" s="207"/>
+      <c r="C20" s="210"/>
       <c r="D20" s="26" t="s">
         <v>481</v>
       </c>
@@ -10785,9 +10785,9 @@
       <c r="W20" s="9"/>
     </row>
     <row r="21" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A21" s="214"/>
-      <c r="B21" s="186"/>
-      <c r="C21" s="177"/>
+      <c r="A21" s="234"/>
+      <c r="B21" s="207"/>
+      <c r="C21" s="210"/>
       <c r="D21" s="26" t="s">
         <v>481</v>
       </c>
@@ -10834,9 +10834,9 @@
       <c r="W21" s="9"/>
     </row>
     <row r="22" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A22" s="215"/>
-      <c r="B22" s="187"/>
-      <c r="C22" s="178"/>
+      <c r="A22" s="235"/>
+      <c r="B22" s="208"/>
+      <c r="C22" s="211"/>
       <c r="D22" s="26" t="s">
         <v>481</v>
       </c>
@@ -11077,10 +11077,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="233" t="s">
         <v>534</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="206" t="s">
         <v>582</v>
       </c>
       <c r="C2" s="26" t="s">
@@ -11142,8 +11142,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" s="12" customFormat="1" ht="56.25" customHeight="1">
-      <c r="A3" s="214"/>
-      <c r="B3" s="186"/>
+      <c r="A3" s="234"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="23" t="s">
         <v>583</v>
       </c>
@@ -11203,8 +11203,8 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A4" s="214"/>
-      <c r="B4" s="186"/>
+      <c r="A4" s="234"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="26" t="s">
         <v>487</v>
       </c>
@@ -11264,9 +11264,9 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A5" s="214"/>
-      <c r="B5" s="186"/>
-      <c r="C5" s="203" t="s">
+      <c r="A5" s="234"/>
+      <c r="B5" s="207"/>
+      <c r="C5" s="225" t="s">
         <v>586</v>
       </c>
       <c r="D5" s="26" t="s">
@@ -11325,9 +11325,9 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A6" s="214"/>
-      <c r="B6" s="186"/>
-      <c r="C6" s="203"/>
+      <c r="A6" s="234"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="225"/>
       <c r="D6" s="26" t="s">
         <v>481</v>
       </c>
@@ -11384,9 +11384,9 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="214"/>
-      <c r="B7" s="186"/>
-      <c r="C7" s="216" t="s">
+      <c r="A7" s="234"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="236" t="s">
         <v>587</v>
       </c>
       <c r="D7" s="26" t="s">
@@ -11445,9 +11445,9 @@
       </c>
     </row>
     <row r="8" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A8" s="214"/>
-      <c r="B8" s="186"/>
-      <c r="C8" s="216"/>
+      <c r="A8" s="234"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="236"/>
       <c r="D8" s="26" t="s">
         <v>481</v>
       </c>
@@ -11504,9 +11504,9 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A9" s="214"/>
-      <c r="B9" s="186"/>
-      <c r="C9" s="216"/>
+      <c r="A9" s="234"/>
+      <c r="B9" s="207"/>
+      <c r="C9" s="236"/>
       <c r="D9" s="26" t="s">
         <v>481</v>
       </c>
@@ -11563,9 +11563,9 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A10" s="214"/>
-      <c r="B10" s="186"/>
-      <c r="C10" s="216"/>
+      <c r="A10" s="234"/>
+      <c r="B10" s="207"/>
+      <c r="C10" s="236"/>
       <c r="D10" s="26" t="s">
         <v>481</v>
       </c>
@@ -11614,9 +11614,9 @@
       <c r="W10" s="64"/>
     </row>
     <row r="11" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A11" s="214"/>
-      <c r="B11" s="186"/>
-      <c r="C11" s="216"/>
+      <c r="A11" s="234"/>
+      <c r="B11" s="207"/>
+      <c r="C11" s="236"/>
       <c r="D11" s="26" t="s">
         <v>481</v>
       </c>
@@ -11665,9 +11665,9 @@
       <c r="W11" s="64"/>
     </row>
     <row r="12" spans="1:23" ht="27" customHeight="1">
-      <c r="A12" s="214"/>
-      <c r="B12" s="186"/>
-      <c r="C12" s="216"/>
+      <c r="A12" s="234"/>
+      <c r="B12" s="207"/>
+      <c r="C12" s="236"/>
       <c r="D12" s="26" t="s">
         <v>481</v>
       </c>
@@ -11714,9 +11714,9 @@
       <c r="W12" s="64"/>
     </row>
     <row r="13" spans="1:23" ht="27" customHeight="1">
-      <c r="A13" s="214"/>
-      <c r="B13" s="186"/>
-      <c r="C13" s="216"/>
+      <c r="A13" s="234"/>
+      <c r="B13" s="207"/>
+      <c r="C13" s="236"/>
       <c r="D13" s="26" t="s">
         <v>481</v>
       </c>
@@ -11763,9 +11763,9 @@
       <c r="W13" s="64"/>
     </row>
     <row r="14" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A14" s="214"/>
-      <c r="B14" s="186"/>
-      <c r="C14" s="216"/>
+      <c r="A14" s="234"/>
+      <c r="B14" s="207"/>
+      <c r="C14" s="236"/>
       <c r="D14" s="26" t="s">
         <v>481</v>
       </c>
@@ -11822,9 +11822,9 @@
       </c>
     </row>
     <row r="15" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A15" s="214"/>
-      <c r="B15" s="186"/>
-      <c r="C15" s="216"/>
+      <c r="A15" s="234"/>
+      <c r="B15" s="207"/>
+      <c r="C15" s="236"/>
       <c r="D15" s="23" t="s">
         <v>481</v>
       </c>
@@ -11881,9 +11881,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A16" s="214"/>
-      <c r="B16" s="186"/>
-      <c r="C16" s="216"/>
+      <c r="A16" s="234"/>
+      <c r="B16" s="207"/>
+      <c r="C16" s="236"/>
       <c r="D16" s="26" t="s">
         <v>481</v>
       </c>
@@ -11940,9 +11940,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A17" s="214"/>
-      <c r="B17" s="186"/>
-      <c r="C17" s="216" t="s">
+      <c r="A17" s="234"/>
+      <c r="B17" s="207"/>
+      <c r="C17" s="236" t="s">
         <v>588</v>
       </c>
       <c r="D17" s="26" t="s">
@@ -12001,9 +12001,9 @@
       </c>
     </row>
     <row r="18" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A18" s="214"/>
-      <c r="B18" s="186"/>
-      <c r="C18" s="216"/>
+      <c r="A18" s="234"/>
+      <c r="B18" s="207"/>
+      <c r="C18" s="236"/>
       <c r="D18" s="26" t="s">
         <v>481</v>
       </c>
@@ -12060,9 +12060,9 @@
       </c>
     </row>
     <row r="19" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A19" s="214"/>
-      <c r="B19" s="186"/>
-      <c r="C19" s="216"/>
+      <c r="A19" s="234"/>
+      <c r="B19" s="207"/>
+      <c r="C19" s="236"/>
       <c r="D19" s="26" t="s">
         <v>481</v>
       </c>
@@ -12119,9 +12119,9 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="27" customHeight="1">
-      <c r="A20" s="214"/>
-      <c r="B20" s="186"/>
-      <c r="C20" s="216"/>
+      <c r="A20" s="234"/>
+      <c r="B20" s="207"/>
+      <c r="C20" s="236"/>
       <c r="D20" s="26" t="s">
         <v>481</v>
       </c>
@@ -12170,9 +12170,9 @@
       <c r="W20" s="64"/>
     </row>
     <row r="21" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A21" s="214"/>
-      <c r="B21" s="186"/>
-      <c r="C21" s="216"/>
+      <c r="A21" s="234"/>
+      <c r="B21" s="207"/>
+      <c r="C21" s="236"/>
       <c r="D21" s="26" t="s">
         <v>481</v>
       </c>
@@ -12221,9 +12221,9 @@
       <c r="W21" s="64"/>
     </row>
     <row r="22" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A22" s="214"/>
-      <c r="B22" s="186"/>
-      <c r="C22" s="216"/>
+      <c r="A22" s="234"/>
+      <c r="B22" s="207"/>
+      <c r="C22" s="236"/>
       <c r="D22" s="26" t="s">
         <v>481</v>
       </c>
@@ -12270,9 +12270,9 @@
       <c r="W22" s="64"/>
     </row>
     <row r="23" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A23" s="214"/>
-      <c r="B23" s="186"/>
-      <c r="C23" s="216"/>
+      <c r="A23" s="234"/>
+      <c r="B23" s="207"/>
+      <c r="C23" s="236"/>
       <c r="D23" s="26" t="s">
         <v>481</v>
       </c>
@@ -12319,9 +12319,9 @@
       <c r="W23" s="64"/>
     </row>
     <row r="24" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A24" s="214"/>
-      <c r="B24" s="186"/>
-      <c r="C24" s="216"/>
+      <c r="A24" s="234"/>
+      <c r="B24" s="207"/>
+      <c r="C24" s="236"/>
       <c r="D24" s="26" t="s">
         <v>481</v>
       </c>
@@ -12378,9 +12378,9 @@
       </c>
     </row>
     <row r="25" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A25" s="214"/>
-      <c r="B25" s="186"/>
-      <c r="C25" s="216"/>
+      <c r="A25" s="234"/>
+      <c r="B25" s="207"/>
+      <c r="C25" s="236"/>
       <c r="D25" s="26" t="s">
         <v>481</v>
       </c>
@@ -12437,9 +12437,9 @@
       </c>
     </row>
     <row r="26" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A26" s="215"/>
-      <c r="B26" s="187"/>
-      <c r="C26" s="216"/>
+      <c r="A26" s="235"/>
+      <c r="B26" s="208"/>
+      <c r="C26" s="236"/>
       <c r="D26" s="26" t="s">
         <v>481</v>
       </c>
@@ -13036,25 +13036,25 @@
       <c r="Q12" s="9"/>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="223" t="s">
+      <c r="A25" s="243" t="s">
         <v>243</v>
       </c>
-      <c r="B25" s="223"/>
-      <c r="C25" s="223"/>
-      <c r="D25" s="223"/>
-      <c r="E25" s="223"/>
-      <c r="F25" s="223"/>
-      <c r="G25" s="223"/>
-      <c r="H25" s="223"/>
-      <c r="I25" s="223"/>
-      <c r="J25" s="223"/>
-      <c r="K25" s="223"/>
-      <c r="L25" s="223"/>
-      <c r="M25" s="223"/>
-      <c r="N25" s="223"/>
-      <c r="O25" s="223"/>
-      <c r="P25" s="223"/>
-      <c r="Q25" s="223"/>
+      <c r="B25" s="243"/>
+      <c r="C25" s="243"/>
+      <c r="D25" s="243"/>
+      <c r="E25" s="243"/>
+      <c r="F25" s="243"/>
+      <c r="G25" s="243"/>
+      <c r="H25" s="243"/>
+      <c r="I25" s="243"/>
+      <c r="J25" s="243"/>
+      <c r="K25" s="243"/>
+      <c r="L25" s="243"/>
+      <c r="M25" s="243"/>
+      <c r="N25" s="243"/>
+      <c r="O25" s="243"/>
+      <c r="P25" s="243"/>
+      <c r="Q25" s="243"/>
       <c r="R25" s="20"/>
       <c r="S25" s="20"/>
       <c r="T25" s="2"/>
@@ -13063,13 +13063,13 @@
       <c r="W25" s="8"/>
     </row>
     <row r="26" spans="1:23" ht="240">
-      <c r="A26" s="224" t="s">
+      <c r="A26" s="244" t="s">
         <v>487</v>
       </c>
-      <c r="B26" s="185" t="s">
+      <c r="B26" s="206" t="s">
         <v>487</v>
       </c>
-      <c r="C26" s="210" t="s">
+      <c r="C26" s="218" t="s">
         <v>487</v>
       </c>
       <c r="D26" s="35" t="s">
@@ -13122,9 +13122,9 @@
       <c r="W26" s="8"/>
     </row>
     <row r="27" spans="1:23" ht="409.5">
-      <c r="A27" s="224"/>
-      <c r="B27" s="186"/>
-      <c r="C27" s="211"/>
+      <c r="A27" s="244"/>
+      <c r="B27" s="207"/>
+      <c r="C27" s="232"/>
       <c r="D27" s="35" t="s">
         <v>518</v>
       </c>
@@ -13173,9 +13173,9 @@
       <c r="W27" s="8"/>
     </row>
     <row r="28" spans="1:23" ht="270">
-      <c r="A28" s="224"/>
-      <c r="B28" s="186"/>
-      <c r="C28" s="211"/>
+      <c r="A28" s="244"/>
+      <c r="B28" s="207"/>
+      <c r="C28" s="232"/>
       <c r="D28" s="35" t="s">
         <v>518</v>
       </c>
@@ -13228,9 +13228,9 @@
       <c r="W28" s="8"/>
     </row>
     <row r="29" spans="1:23" ht="285">
-      <c r="A29" s="224"/>
-      <c r="B29" s="186"/>
-      <c r="C29" s="211"/>
+      <c r="A29" s="244"/>
+      <c r="B29" s="207"/>
+      <c r="C29" s="232"/>
       <c r="D29" s="35" t="s">
         <v>518</v>
       </c>
@@ -13281,9 +13281,9 @@
       <c r="W29" s="8"/>
     </row>
     <row r="30" spans="1:23" ht="360">
-      <c r="A30" s="224"/>
-      <c r="B30" s="186"/>
-      <c r="C30" s="211"/>
+      <c r="A30" s="244"/>
+      <c r="B30" s="207"/>
+      <c r="C30" s="232"/>
       <c r="D30" s="35" t="s">
         <v>518</v>
       </c>
@@ -13334,9 +13334,9 @@
       <c r="W30" s="20"/>
     </row>
     <row r="31" spans="1:23" ht="409.5">
-      <c r="A31" s="224"/>
-      <c r="B31" s="186"/>
-      <c r="C31" s="211"/>
+      <c r="A31" s="244"/>
+      <c r="B31" s="207"/>
+      <c r="C31" s="232"/>
       <c r="D31" s="35" t="s">
         <v>518</v>
       </c>
@@ -13387,9 +13387,9 @@
       <c r="W31" s="8"/>
     </row>
     <row r="32" spans="1:23" ht="409.5">
-      <c r="A32" s="224"/>
-      <c r="B32" s="187"/>
-      <c r="C32" s="212"/>
+      <c r="A32" s="244"/>
+      <c r="B32" s="208"/>
+      <c r="C32" s="219"/>
       <c r="D32" s="35" t="s">
         <v>518</v>
       </c>
@@ -13484,77 +13484,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2685157-6CD4-4E90-8A5D-0A2DE42DCE28}">
   <dimension ref="C1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="30" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="228" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="130" customWidth="1"/>
     <col min="5" max="5" width="44.5703125" style="31" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" style="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" style="31" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" s="149" customFormat="1" ht="16.5" thickBot="1"/>
+    <row r="1" spans="3:7" s="173" customFormat="1" ht="16.5" thickBot="1"/>
     <row r="2" spans="3:7" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C2" s="156" t="s">
+      <c r="C2" s="180" t="s">
         <v>517</v>
       </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
-      <c r="G2" s="158"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="182"/>
     </row>
     <row r="3" spans="3:7" ht="16.5" thickBot="1">
-      <c r="C3" s="159"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="161"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="185"/>
     </row>
     <row r="4" spans="3:7" ht="19.5" customHeight="1" thickBot="1">
-      <c r="C4" s="236" t="s">
+      <c r="C4" s="245" t="s">
         <v>959</v>
       </c>
-      <c r="D4" s="237"/>
-      <c r="E4" s="233" t="s">
+      <c r="D4" s="246"/>
+      <c r="E4" s="135" t="s">
         <v>962</v>
       </c>
-      <c r="F4" s="234" t="s">
+      <c r="F4" s="165" t="s">
         <v>960</v>
       </c>
-      <c r="G4" s="235"/>
+      <c r="G4" s="166"/>
     </row>
     <row r="5" spans="3:7" ht="16.5" thickBot="1">
-      <c r="C5" s="162"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="C5" s="186"/>
+      <c r="D5" s="187"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="187"/>
+      <c r="G5" s="188"/>
     </row>
     <row r="6" spans="3:7" ht="18.75" customHeight="1">
-      <c r="C6" s="169" t="s">
+      <c r="C6" s="193" t="s">
         <v>507</v>
       </c>
-      <c r="D6" s="167" t="s">
+      <c r="D6" s="191" t="s">
         <v>535</v>
       </c>
-      <c r="E6" s="165" t="s">
+      <c r="E6" s="189" t="s">
         <v>663</v>
       </c>
-      <c r="F6" s="167" t="s">
+      <c r="F6" s="191" t="s">
         <v>652</v>
       </c>
-      <c r="G6" s="171"/>
+      <c r="G6" s="195"/>
     </row>
     <row r="7" spans="3:7" ht="16.5" thickBot="1">
-      <c r="C7" s="170"/>
-      <c r="D7" s="168"/>
-      <c r="E7" s="166"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="190"/>
       <c r="F7" s="112" t="s">
         <v>669</v>
       </c>
@@ -13566,10 +13566,10 @@
       <c r="C8" s="109">
         <v>1</v>
       </c>
-      <c r="D8" s="225" t="s">
+      <c r="D8" s="127" t="s">
         <v>524</v>
       </c>
-      <c r="E8" s="229" t="s">
+      <c r="E8" s="131" t="s">
         <v>523</v>
       </c>
       <c r="F8" s="110">
@@ -13583,10 +13583,10 @@
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="D9" s="226" t="s">
+      <c r="D9" s="128" t="s">
         <v>525</v>
       </c>
-      <c r="E9" s="230" t="s">
+      <c r="E9" s="132" t="s">
         <v>508</v>
       </c>
       <c r="F9" s="81">
@@ -13600,10 +13600,10 @@
       <c r="C10" s="32">
         <v>3</v>
       </c>
-      <c r="D10" s="226" t="s">
+      <c r="D10" s="128" t="s">
         <v>526</v>
       </c>
-      <c r="E10" s="231" t="s">
+      <c r="E10" s="133" t="s">
         <v>522</v>
       </c>
       <c r="F10" s="80">
@@ -13617,10 +13617,10 @@
       <c r="C11" s="32">
         <v>4</v>
       </c>
-      <c r="D11" s="226" t="s">
+      <c r="D11" s="128" t="s">
         <v>527</v>
       </c>
-      <c r="E11" s="230" t="s">
+      <c r="E11" s="132" t="s">
         <v>509</v>
       </c>
       <c r="F11" s="81">
@@ -13634,10 +13634,10 @@
       <c r="C12" s="32">
         <v>5</v>
       </c>
-      <c r="D12" s="226" t="s">
+      <c r="D12" s="128" t="s">
         <v>528</v>
       </c>
-      <c r="E12" s="230" t="s">
+      <c r="E12" s="132" t="s">
         <v>510</v>
       </c>
       <c r="F12" s="81">
@@ -13651,10 +13651,10 @@
       <c r="C13" s="32">
         <v>6</v>
       </c>
-      <c r="D13" s="226" t="s">
+      <c r="D13" s="128" t="s">
         <v>529</v>
       </c>
-      <c r="E13" s="230" t="s">
+      <c r="E13" s="132" t="s">
         <v>511</v>
       </c>
       <c r="F13" s="81">
@@ -13668,10 +13668,10 @@
       <c r="C14" s="32">
         <v>7</v>
       </c>
-      <c r="D14" s="226" t="s">
+      <c r="D14" s="128" t="s">
         <v>530</v>
       </c>
-      <c r="E14" s="230" t="s">
+      <c r="E14" s="132" t="s">
         <v>512</v>
       </c>
       <c r="F14" s="81">
@@ -13685,10 +13685,10 @@
       <c r="C15" s="32">
         <v>8</v>
       </c>
-      <c r="D15" s="226" t="s">
+      <c r="D15" s="128" t="s">
         <v>531</v>
       </c>
-      <c r="E15" s="230" t="s">
+      <c r="E15" s="132" t="s">
         <v>513</v>
       </c>
       <c r="F15" s="81">
@@ -13702,10 +13702,10 @@
       <c r="C16" s="32">
         <v>9</v>
       </c>
-      <c r="D16" s="226" t="s">
+      <c r="D16" s="128" t="s">
         <v>532</v>
       </c>
-      <c r="E16" s="230" t="s">
+      <c r="E16" s="132" t="s">
         <v>514</v>
       </c>
       <c r="F16" s="81">
@@ -13719,10 +13719,10 @@
       <c r="C17" s="32">
         <v>10</v>
       </c>
-      <c r="D17" s="226" t="s">
+      <c r="D17" s="128" t="s">
         <v>533</v>
       </c>
-      <c r="E17" s="230" t="s">
+      <c r="E17" s="132" t="s">
         <v>515</v>
       </c>
       <c r="F17" s="81">
@@ -13736,10 +13736,10 @@
       <c r="C18" s="32">
         <v>11</v>
       </c>
-      <c r="D18" s="226" t="s">
+      <c r="D18" s="128" t="s">
         <v>534</v>
       </c>
-      <c r="E18" s="230" t="s">
+      <c r="E18" s="132" t="s">
         <v>516</v>
       </c>
       <c r="F18" s="81">
@@ -13751,23 +13751,23 @@
     </row>
     <row r="19" spans="3:7" ht="16.5" thickBot="1">
       <c r="C19" s="114"/>
-      <c r="D19" s="227"/>
-      <c r="E19" s="232"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="134"/>
       <c r="F19" s="106"/>
       <c r="G19" s="107"/>
     </row>
     <row r="20" spans="3:7" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="C20" s="150"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="152"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="175"/>
+      <c r="E20" s="176"/>
       <c r="F20" s="120"/>
       <c r="G20" s="121"/>
     </row>
     <row r="21" spans="3:7" ht="16.5" customHeight="1">
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="161" t="s">
         <v>958</v>
       </c>
-      <c r="D21" s="173"/>
+      <c r="D21" s="162"/>
       <c r="E21" s="115" t="s">
         <v>956</v>
       </c>
@@ -13779,8 +13779,8 @@
       </c>
     </row>
     <row r="22" spans="3:7" ht="16.5" thickBot="1">
-      <c r="C22" s="174"/>
-      <c r="D22" s="175"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="164"/>
       <c r="E22" s="117">
         <v>163</v>
       </c>
@@ -13792,18 +13792,18 @@
       </c>
     </row>
     <row r="23" spans="3:7" ht="16.5" thickBot="1">
-      <c r="C23" s="153"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="155"/>
-    </row>
-    <row r="24" spans="3:7" s="149" customFormat="1" ht="16.5" thickBot="1"/>
+      <c r="C23" s="177"/>
+      <c r="D23" s="178"/>
+      <c r="E23" s="178"/>
+      <c r="F23" s="178"/>
+      <c r="G23" s="179"/>
+    </row>
+    <row r="24" spans="3:7" s="173" customFormat="1" ht="16.5" thickBot="1"/>
     <row r="25" spans="3:7" ht="16.5" thickBot="1">
-      <c r="F25" s="143" t="s">
+      <c r="F25" s="167" t="s">
         <v>666</v>
       </c>
-      <c r="G25" s="144"/>
+      <c r="G25" s="168"/>
     </row>
     <row r="26" spans="3:7" ht="16.5" thickBot="1">
       <c r="F26" s="122" t="s">
@@ -13822,24 +13822,19 @@
       </c>
     </row>
     <row r="28" spans="3:7" ht="16.5" thickBot="1">
-      <c r="F28" s="145" t="s">
+      <c r="F28" s="169" t="s">
         <v>667</v>
       </c>
-      <c r="G28" s="146"/>
+      <c r="G28" s="170"/>
     </row>
     <row r="29" spans="3:7" ht="17.25" thickTop="1" thickBot="1">
-      <c r="F29" s="147">
+      <c r="F29" s="171">
         <v>163</v>
       </c>
-      <c r="G29" s="148"/>
+      <c r="G29" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="A24:XFD24"/>
@@ -13852,6 +13847,11 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F25:F26 F28:F29">
@@ -13913,7 +13913,7 @@
     <hyperlink ref="D14" location="'Assets Group'!A1" display="AMS_MD_7" xr:uid="{01F4E7AF-D6A1-4D1E-8497-37914AD62E6C}"/>
     <hyperlink ref="D17" location="'Asset Status'!A1" display="AMS_MD_10" xr:uid="{96F13612-B64A-4B60-BB15-00FD0D1C1DAF}"/>
     <hyperlink ref="D18" location="'User Module'!A1" display="AMS_MD_11" xr:uid="{82CFEEC2-B19E-41DA-B7FC-52079DFBE425}"/>
-    <hyperlink ref="C4:D4" location="'Project Profile'!B3" display="Go Back To The Project Profile" xr:uid="{543066F6-B863-4246-85CA-19B654935B60}"/>
+    <hyperlink ref="C4:D4" location="'Project Profile'!C3" display="Go Back To The Project Profile" xr:uid="{543066F6-B863-4246-85CA-19B654935B60}"/>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{066D2424-EC25-4A29-8216-796A3D623214}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14076,10 +14076,10 @@
       <c r="W2" s="52"/>
     </row>
     <row r="3" spans="1:53" ht="120">
-      <c r="A3" s="188" t="s">
+      <c r="A3" s="196" t="s">
         <v>524</v>
       </c>
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="215" t="s">
         <v>470</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -14135,9 +14135,9 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:53" ht="15" customHeight="1">
-      <c r="A4" s="189"/>
-      <c r="B4" s="183"/>
-      <c r="C4" s="210" t="s">
+      <c r="A4" s="197"/>
+      <c r="B4" s="216"/>
+      <c r="C4" s="218" t="s">
         <v>487</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -14188,9 +14188,9 @@
       <c r="W4" s="20"/>
     </row>
     <row r="5" spans="1:53" ht="15" customHeight="1">
-      <c r="A5" s="189"/>
-      <c r="B5" s="183"/>
-      <c r="C5" s="212"/>
+      <c r="A5" s="197"/>
+      <c r="B5" s="216"/>
+      <c r="C5" s="219"/>
       <c r="D5" s="21" t="s">
         <v>518</v>
       </c>
@@ -14237,9 +14237,9 @@
       <c r="W5" s="8"/>
     </row>
     <row r="6" spans="1:53" ht="30">
-      <c r="A6" s="189"/>
-      <c r="B6" s="183"/>
-      <c r="C6" s="179" t="s">
+      <c r="A6" s="197"/>
+      <c r="B6" s="216"/>
+      <c r="C6" s="212" t="s">
         <v>473</v>
       </c>
       <c r="D6" s="26" t="s">
@@ -14292,9 +14292,9 @@
       <c r="W6" s="7"/>
     </row>
     <row r="7" spans="1:53" ht="30">
-      <c r="A7" s="189"/>
-      <c r="B7" s="183"/>
-      <c r="C7" s="180"/>
+      <c r="A7" s="197"/>
+      <c r="B7" s="216"/>
+      <c r="C7" s="213"/>
       <c r="D7" s="26" t="s">
         <v>481</v>
       </c>
@@ -14345,9 +14345,9 @@
       <c r="W7" s="8"/>
     </row>
     <row r="8" spans="1:53" ht="45">
-      <c r="A8" s="189"/>
-      <c r="B8" s="183"/>
-      <c r="C8" s="180"/>
+      <c r="A8" s="197"/>
+      <c r="B8" s="216"/>
+      <c r="C8" s="213"/>
       <c r="D8" s="26" t="s">
         <v>481</v>
       </c>
@@ -14400,9 +14400,9 @@
       <c r="W8" s="20"/>
     </row>
     <row r="9" spans="1:53" ht="30">
-      <c r="A9" s="190"/>
-      <c r="B9" s="184"/>
-      <c r="C9" s="181"/>
+      <c r="A9" s="198"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="214"/>
       <c r="D9" s="26" t="s">
         <v>481</v>
       </c>
@@ -14453,13 +14453,13 @@
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:53" ht="38.25" customHeight="1">
-      <c r="A10" s="191" t="s">
+      <c r="A10" s="199" t="s">
         <v>525</v>
       </c>
-      <c r="B10" s="196" t="s">
+      <c r="B10" s="204" t="s">
         <v>474</v>
       </c>
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="212" t="s">
         <v>477</v>
       </c>
       <c r="D10" s="23" t="s">
@@ -14512,9 +14512,9 @@
       <c r="W10" s="7"/>
     </row>
     <row r="11" spans="1:53" ht="38.25" customHeight="1">
-      <c r="A11" s="192"/>
-      <c r="B11" s="197"/>
-      <c r="C11" s="181"/>
+      <c r="A11" s="200"/>
+      <c r="B11" s="205"/>
+      <c r="C11" s="214"/>
       <c r="D11" s="23" t="s">
         <v>481</v>
       </c>
@@ -14624,10 +14624,10 @@
       <c r="BA12" s="53"/>
     </row>
     <row r="13" spans="1:53" ht="30">
-      <c r="A13" s="193" t="s">
+      <c r="A13" s="201" t="s">
         <v>524</v>
       </c>
-      <c r="B13" s="185" t="s">
+      <c r="B13" s="206" t="s">
         <v>470</v>
       </c>
       <c r="C13" s="26" t="s">
@@ -14685,9 +14685,9 @@
       <c r="W13" s="9"/>
     </row>
     <row r="14" spans="1:53" ht="30">
-      <c r="A14" s="194"/>
-      <c r="B14" s="186"/>
-      <c r="C14" s="176" t="s">
+      <c r="A14" s="202"/>
+      <c r="B14" s="207"/>
+      <c r="C14" s="209" t="s">
         <v>476</v>
       </c>
       <c r="D14" s="26" t="s">
@@ -14740,9 +14740,9 @@
       <c r="W14" s="9"/>
     </row>
     <row r="15" spans="1:53" ht="30">
-      <c r="A15" s="194"/>
-      <c r="B15" s="186"/>
-      <c r="C15" s="177"/>
+      <c r="A15" s="202"/>
+      <c r="B15" s="207"/>
+      <c r="C15" s="210"/>
       <c r="D15" s="26" t="s">
         <v>481</v>
       </c>
@@ -14793,9 +14793,9 @@
       <c r="W15" s="9"/>
     </row>
     <row r="16" spans="1:53" ht="30">
-      <c r="A16" s="194"/>
-      <c r="B16" s="186"/>
-      <c r="C16" s="178"/>
+      <c r="A16" s="202"/>
+      <c r="B16" s="207"/>
+      <c r="C16" s="211"/>
       <c r="D16" s="26" t="s">
         <v>481</v>
       </c>
@@ -14846,8 +14846,8 @@
       <c r="W16" s="9"/>
     </row>
     <row r="17" spans="1:53" ht="30">
-      <c r="A17" s="195"/>
-      <c r="B17" s="187"/>
+      <c r="A17" s="203"/>
+      <c r="B17" s="208"/>
       <c r="C17" s="77" t="s">
         <v>653</v>
       </c>
@@ -14956,10 +14956,10 @@
       <c r="BA18" s="53"/>
     </row>
     <row r="19" spans="1:53" ht="26.25" customHeight="1">
-      <c r="A19" s="193" t="s">
+      <c r="A19" s="201" t="s">
         <v>525</v>
       </c>
-      <c r="B19" s="185" t="s">
+      <c r="B19" s="206" t="s">
         <v>474</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -15015,9 +15015,9 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20" spans="1:53" ht="15" customHeight="1">
-      <c r="A20" s="194"/>
-      <c r="B20" s="186"/>
-      <c r="C20" s="210" t="s">
+      <c r="A20" s="202"/>
+      <c r="B20" s="207"/>
+      <c r="C20" s="218" t="s">
         <v>487</v>
       </c>
       <c r="D20" s="21" t="s">
@@ -15072,9 +15072,9 @@
       <c r="W20" s="20"/>
     </row>
     <row r="21" spans="1:53" ht="15" customHeight="1">
-      <c r="A21" s="194"/>
-      <c r="B21" s="186"/>
-      <c r="C21" s="212"/>
+      <c r="A21" s="202"/>
+      <c r="B21" s="207"/>
+      <c r="C21" s="219"/>
       <c r="D21" s="21" t="s">
         <v>518</v>
       </c>
@@ -15125,9 +15125,9 @@
       <c r="W21" s="20"/>
     </row>
     <row r="22" spans="1:53" ht="26.25" customHeight="1">
-      <c r="A22" s="194"/>
-      <c r="B22" s="186"/>
-      <c r="C22" s="176" t="s">
+      <c r="A22" s="202"/>
+      <c r="B22" s="207"/>
+      <c r="C22" s="209" t="s">
         <v>477</v>
       </c>
       <c r="D22" s="26" t="s">
@@ -15180,9 +15180,9 @@
       <c r="W22" s="9"/>
     </row>
     <row r="23" spans="1:53" ht="45">
-      <c r="A23" s="194"/>
-      <c r="B23" s="186"/>
-      <c r="C23" s="177"/>
+      <c r="A23" s="202"/>
+      <c r="B23" s="207"/>
+      <c r="C23" s="210"/>
       <c r="D23" s="26" t="s">
         <v>481</v>
       </c>
@@ -15233,9 +15233,9 @@
       <c r="W23" s="9"/>
     </row>
     <row r="24" spans="1:53" ht="26.25" customHeight="1">
-      <c r="A24" s="194"/>
-      <c r="B24" s="186"/>
-      <c r="C24" s="178"/>
+      <c r="A24" s="202"/>
+      <c r="B24" s="207"/>
+      <c r="C24" s="211"/>
       <c r="D24" s="26" t="s">
         <v>481</v>
       </c>
@@ -15288,8 +15288,8 @@
       <c r="W24" s="9"/>
     </row>
     <row r="25" spans="1:53" ht="26.25" customHeight="1">
-      <c r="A25" s="195"/>
-      <c r="B25" s="187"/>
+      <c r="A25" s="203"/>
+      <c r="B25" s="208"/>
       <c r="C25" s="26" t="s">
         <v>478</v>
       </c>
@@ -18472,12 +18472,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="C10:C11"/>
@@ -18486,6 +18480,12 @@
     <mergeCell ref="B19:B25"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D1:D30 D36:D1048576">
@@ -18691,10 +18691,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="115.5" customHeight="1">
-      <c r="A2" s="198" t="s">
+      <c r="A2" s="220" t="s">
         <v>526</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="206" t="s">
         <v>486</v>
       </c>
       <c r="C2" s="26" t="s">
@@ -18752,8 +18752,8 @@
       <c r="W2" s="7"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="90">
-      <c r="A3" s="199"/>
-      <c r="B3" s="186"/>
+      <c r="A3" s="221"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="26" t="s">
         <v>601</v>
       </c>
@@ -18807,8 +18807,8 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="75">
-      <c r="A4" s="199"/>
-      <c r="B4" s="186"/>
+      <c r="A4" s="221"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="26" t="s">
         <v>602</v>
       </c>
@@ -18864,8 +18864,8 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="180">
-      <c r="A5" s="200"/>
-      <c r="B5" s="187"/>
+      <c r="A5" s="222"/>
+      <c r="B5" s="208"/>
       <c r="C5" s="35" t="s">
         <v>699</v>
       </c>
@@ -19061,13 +19061,13 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="75">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="224" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="223" t="s">
         <v>538</v>
       </c>
-      <c r="C2" s="203" t="s">
+      <c r="C2" s="225" t="s">
         <v>661</v>
       </c>
       <c r="D2" s="35" t="s">
@@ -19120,9 +19120,9 @@
       <c r="W2" s="8"/>
     </row>
     <row r="3" spans="1:23" ht="45.75" customHeight="1">
-      <c r="A3" s="202"/>
-      <c r="B3" s="201"/>
-      <c r="C3" s="203"/>
+      <c r="A3" s="224"/>
+      <c r="B3" s="223"/>
+      <c r="C3" s="225"/>
       <c r="D3" s="35" t="s">
         <v>481</v>
       </c>
@@ -19173,9 +19173,9 @@
       <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" ht="43.5" customHeight="1">
-      <c r="A4" s="202"/>
-      <c r="B4" s="201"/>
-      <c r="C4" s="203"/>
+      <c r="A4" s="224"/>
+      <c r="B4" s="223"/>
+      <c r="C4" s="225"/>
       <c r="D4" s="35" t="s">
         <v>481</v>
       </c>
@@ -19228,9 +19228,9 @@
       <c r="W4" s="8"/>
     </row>
     <row r="5" spans="1:23" ht="36.75" customHeight="1">
-      <c r="A5" s="202"/>
-      <c r="B5" s="201"/>
-      <c r="C5" s="203"/>
+      <c r="A5" s="224"/>
+      <c r="B5" s="223"/>
+      <c r="C5" s="225"/>
       <c r="D5" s="35" t="s">
         <v>518</v>
       </c>
@@ -19281,9 +19281,9 @@
       <c r="W5" s="8"/>
     </row>
     <row r="6" spans="1:23" ht="38.25" customHeight="1">
-      <c r="A6" s="202"/>
-      <c r="B6" s="201"/>
-      <c r="C6" s="203"/>
+      <c r="A6" s="224"/>
+      <c r="B6" s="223"/>
+      <c r="C6" s="225"/>
       <c r="D6" s="35" t="s">
         <v>518</v>
       </c>
@@ -19334,9 +19334,9 @@
       <c r="W6" s="8"/>
     </row>
     <row r="7" spans="1:23" ht="30.75" customHeight="1">
-      <c r="A7" s="202"/>
-      <c r="B7" s="201"/>
-      <c r="C7" s="203"/>
+      <c r="A7" s="224"/>
+      <c r="B7" s="223"/>
+      <c r="C7" s="225"/>
       <c r="D7" s="35" t="s">
         <v>518</v>
       </c>
@@ -19387,9 +19387,9 @@
       <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" ht="37.5" customHeight="1">
-      <c r="A8" s="202"/>
-      <c r="B8" s="201"/>
-      <c r="C8" s="203"/>
+      <c r="A8" s="224"/>
+      <c r="B8" s="223"/>
+      <c r="C8" s="225"/>
       <c r="D8" s="35" t="s">
         <v>518</v>
       </c>
@@ -19440,9 +19440,9 @@
       <c r="W8" s="8"/>
     </row>
     <row r="9" spans="1:23" ht="29.25" customHeight="1">
-      <c r="A9" s="202"/>
-      <c r="B9" s="201"/>
-      <c r="C9" s="203"/>
+      <c r="A9" s="224"/>
+      <c r="B9" s="223"/>
+      <c r="C9" s="225"/>
       <c r="D9" s="35" t="s">
         <v>518</v>
       </c>
@@ -19493,8 +19493,8 @@
       <c r="W9" s="8"/>
     </row>
     <row r="10" spans="1:23" ht="53.25" customHeight="1">
-      <c r="A10" s="202"/>
-      <c r="B10" s="201"/>
+      <c r="A10" s="224"/>
+      <c r="B10" s="223"/>
       <c r="C10" s="24" t="s">
         <v>660</v>
       </c>
@@ -19548,8 +19548,8 @@
       <c r="W10" s="8"/>
     </row>
     <row r="11" spans="1:23" ht="34.5" customHeight="1">
-      <c r="A11" s="202"/>
-      <c r="B11" s="201"/>
+      <c r="A11" s="224"/>
+      <c r="B11" s="223"/>
       <c r="C11" s="35" t="s">
         <v>661</v>
       </c>
@@ -19595,8 +19595,8 @@
       <c r="W11" s="8"/>
     </row>
     <row r="12" spans="1:23" ht="35.25" customHeight="1">
-      <c r="A12" s="202"/>
-      <c r="B12" s="201"/>
+      <c r="A12" s="224"/>
+      <c r="B12" s="223"/>
       <c r="C12" s="35" t="s">
         <v>539</v>
       </c>
@@ -19650,9 +19650,9 @@
       <c r="W12" s="8"/>
     </row>
     <row r="13" spans="1:23" ht="36.75" customHeight="1">
-      <c r="A13" s="202"/>
-      <c r="B13" s="201"/>
-      <c r="C13" s="203" t="s">
+      <c r="A13" s="224"/>
+      <c r="B13" s="223"/>
+      <c r="C13" s="225" t="s">
         <v>539</v>
       </c>
       <c r="D13" s="35" t="s">
@@ -19705,9 +19705,9 @@
       <c r="W13" s="8"/>
     </row>
     <row r="14" spans="1:23" ht="36" customHeight="1">
-      <c r="A14" s="202"/>
-      <c r="B14" s="201"/>
-      <c r="C14" s="203"/>
+      <c r="A14" s="224"/>
+      <c r="B14" s="223"/>
+      <c r="C14" s="225"/>
       <c r="D14" s="35" t="s">
         <v>481</v>
       </c>
@@ -19758,9 +19758,9 @@
       <c r="W14" s="8"/>
     </row>
     <row r="15" spans="1:23" ht="36.75" customHeight="1">
-      <c r="A15" s="202"/>
-      <c r="B15" s="201"/>
-      <c r="C15" s="203"/>
+      <c r="A15" s="224"/>
+      <c r="B15" s="223"/>
+      <c r="C15" s="225"/>
       <c r="D15" s="35" t="s">
         <v>518</v>
       </c>
@@ -19811,9 +19811,9 @@
       <c r="W15" s="8"/>
     </row>
     <row r="16" spans="1:23" ht="35.25" customHeight="1">
-      <c r="A16" s="202"/>
-      <c r="B16" s="201"/>
-      <c r="C16" s="203"/>
+      <c r="A16" s="224"/>
+      <c r="B16" s="223"/>
+      <c r="C16" s="225"/>
       <c r="D16" s="35" t="s">
         <v>481</v>
       </c>
@@ -19864,9 +19864,9 @@
       <c r="W16" s="8"/>
     </row>
     <row r="17" spans="1:23" ht="36" customHeight="1">
-      <c r="A17" s="202"/>
-      <c r="B17" s="201"/>
-      <c r="C17" s="203"/>
+      <c r="A17" s="224"/>
+      <c r="B17" s="223"/>
+      <c r="C17" s="225"/>
       <c r="D17" s="35" t="s">
         <v>481</v>
       </c>
@@ -19917,9 +19917,9 @@
       <c r="W17" s="8"/>
     </row>
     <row r="18" spans="1:23" ht="33" customHeight="1">
-      <c r="A18" s="202"/>
-      <c r="B18" s="201"/>
-      <c r="C18" s="203"/>
+      <c r="A18" s="224"/>
+      <c r="B18" s="223"/>
+      <c r="C18" s="225"/>
       <c r="D18" s="35" t="s">
         <v>481</v>
       </c>
@@ -19970,9 +19970,9 @@
       <c r="W18" s="8"/>
     </row>
     <row r="19" spans="1:23" ht="34.5" customHeight="1">
-      <c r="A19" s="202"/>
-      <c r="B19" s="201"/>
-      <c r="C19" s="203"/>
+      <c r="A19" s="224"/>
+      <c r="B19" s="223"/>
+      <c r="C19" s="225"/>
       <c r="D19" s="35" t="s">
         <v>481</v>
       </c>
@@ -20023,9 +20023,9 @@
       <c r="W19" s="8"/>
     </row>
     <row r="20" spans="1:23" ht="36.75" customHeight="1">
-      <c r="A20" s="202"/>
-      <c r="B20" s="201"/>
-      <c r="C20" s="203"/>
+      <c r="A20" s="224"/>
+      <c r="B20" s="223"/>
+      <c r="C20" s="225"/>
       <c r="D20" s="35" t="s">
         <v>481</v>
       </c>
@@ -20076,9 +20076,9 @@
       <c r="W20" s="8"/>
     </row>
     <row r="21" spans="1:23" ht="39" customHeight="1">
-      <c r="A21" s="202"/>
-      <c r="B21" s="201"/>
-      <c r="C21" s="203"/>
+      <c r="A21" s="224"/>
+      <c r="B21" s="223"/>
+      <c r="C21" s="225"/>
       <c r="D21" s="35" t="s">
         <v>481</v>
       </c>
@@ -20129,9 +20129,9 @@
       <c r="W21" s="8"/>
     </row>
     <row r="22" spans="1:23" ht="34.5" customHeight="1">
-      <c r="A22" s="202"/>
-      <c r="B22" s="201"/>
-      <c r="C22" s="203"/>
+      <c r="A22" s="224"/>
+      <c r="B22" s="223"/>
+      <c r="C22" s="225"/>
       <c r="D22" s="35" t="s">
         <v>518</v>
       </c>
@@ -20182,9 +20182,9 @@
       <c r="W22" s="8"/>
     </row>
     <row r="23" spans="1:23" ht="32.25" customHeight="1">
-      <c r="A23" s="202"/>
-      <c r="B23" s="201"/>
-      <c r="C23" s="203"/>
+      <c r="A23" s="224"/>
+      <c r="B23" s="223"/>
+      <c r="C23" s="225"/>
       <c r="D23" s="35" t="s">
         <v>481</v>
       </c>
@@ -20235,9 +20235,9 @@
       <c r="W23" s="8"/>
     </row>
     <row r="24" spans="1:23" ht="36" customHeight="1">
-      <c r="A24" s="202"/>
-      <c r="B24" s="201"/>
-      <c r="C24" s="203"/>
+      <c r="A24" s="224"/>
+      <c r="B24" s="223"/>
+      <c r="C24" s="225"/>
       <c r="D24" s="35" t="s">
         <v>481</v>
       </c>
@@ -20288,9 +20288,9 @@
       <c r="W24" s="8"/>
     </row>
     <row r="25" spans="1:23" ht="27.75" customHeight="1">
-      <c r="A25" s="202"/>
-      <c r="B25" s="201"/>
-      <c r="C25" s="203"/>
+      <c r="A25" s="224"/>
+      <c r="B25" s="223"/>
+      <c r="C25" s="225"/>
       <c r="D25" s="35" t="s">
         <v>481</v>
       </c>
@@ -20341,8 +20341,8 @@
       <c r="W25" s="20"/>
     </row>
     <row r="26" spans="1:23" ht="28.5" customHeight="1">
-      <c r="A26" s="202"/>
-      <c r="B26" s="201"/>
+      <c r="A26" s="224"/>
+      <c r="B26" s="223"/>
       <c r="C26" s="35" t="s">
         <v>662</v>
       </c>
@@ -20539,10 +20539,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="226" t="s">
         <v>528</v>
       </c>
-      <c r="B2" s="206" t="s">
+      <c r="B2" s="228" t="s">
         <v>544</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -20598,8 +20598,8 @@
       <c r="W2" s="8"/>
     </row>
     <row r="3" spans="1:23" ht="46.5" customHeight="1">
-      <c r="A3" s="205"/>
-      <c r="B3" s="207"/>
+      <c r="A3" s="227"/>
+      <c r="B3" s="229"/>
       <c r="C3" s="24" t="s">
         <v>546</v>
       </c>
@@ -20653,8 +20653,8 @@
       <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" ht="33.75" customHeight="1">
-      <c r="A4" s="205"/>
-      <c r="B4" s="207"/>
+      <c r="A4" s="227"/>
+      <c r="B4" s="229"/>
       <c r="C4" s="35" t="s">
         <v>543</v>
       </c>
@@ -20708,8 +20708,8 @@
       <c r="W4" s="8"/>
     </row>
     <row r="5" spans="1:23" ht="32.25" customHeight="1">
-      <c r="A5" s="205"/>
-      <c r="B5" s="207"/>
+      <c r="A5" s="227"/>
+      <c r="B5" s="229"/>
       <c r="C5" s="35" t="s">
         <v>487</v>
       </c>
@@ -20763,8 +20763,8 @@
       <c r="W5" s="8"/>
     </row>
     <row r="6" spans="1:23" ht="23.25" customHeight="1">
-      <c r="A6" s="205"/>
-      <c r="B6" s="207"/>
+      <c r="A6" s="227"/>
+      <c r="B6" s="229"/>
       <c r="C6" s="35" t="s">
         <v>487</v>
       </c>
@@ -20818,8 +20818,8 @@
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23" ht="165">
-      <c r="A7" s="205"/>
-      <c r="B7" s="207"/>
+      <c r="A7" s="227"/>
+      <c r="B7" s="229"/>
       <c r="C7" s="24" t="s">
         <v>548</v>
       </c>
@@ -20873,8 +20873,8 @@
       <c r="W7" s="8"/>
     </row>
     <row r="8" spans="1:23" ht="90">
-      <c r="A8" s="205"/>
-      <c r="B8" s="207"/>
+      <c r="A8" s="227"/>
+      <c r="B8" s="229"/>
       <c r="C8" s="35" t="s">
         <v>543</v>
       </c>
@@ -20924,8 +20924,8 @@
       <c r="W8" s="8"/>
     </row>
     <row r="9" spans="1:23" ht="75">
-      <c r="A9" s="205"/>
-      <c r="B9" s="207"/>
+      <c r="A9" s="227"/>
+      <c r="B9" s="229"/>
       <c r="C9" s="35" t="s">
         <v>547</v>
       </c>
@@ -20979,8 +20979,8 @@
       <c r="W9" s="8"/>
     </row>
     <row r="10" spans="1:23" ht="210">
-      <c r="A10" s="205"/>
-      <c r="B10" s="207"/>
+      <c r="A10" s="227"/>
+      <c r="B10" s="229"/>
       <c r="C10" s="96" t="s">
         <v>547</v>
       </c>
@@ -21034,8 +21034,8 @@
       <c r="W10" s="102"/>
     </row>
     <row r="11" spans="1:23" ht="90">
-      <c r="A11" s="205"/>
-      <c r="B11" s="207"/>
+      <c r="A11" s="227"/>
+      <c r="B11" s="229"/>
       <c r="C11" s="96" t="s">
         <v>547</v>
       </c>
@@ -21091,8 +21091,8 @@
       <c r="W11" s="102"/>
     </row>
     <row r="12" spans="1:23" ht="90">
-      <c r="A12" s="205"/>
-      <c r="B12" s="207"/>
+      <c r="A12" s="227"/>
+      <c r="B12" s="229"/>
       <c r="C12" s="96" t="s">
         <v>547</v>
       </c>
@@ -21148,8 +21148,8 @@
       <c r="W12" s="102"/>
     </row>
     <row r="13" spans="1:23" ht="90">
-      <c r="A13" s="205"/>
-      <c r="B13" s="207"/>
+      <c r="A13" s="227"/>
+      <c r="B13" s="229"/>
       <c r="C13" s="96" t="s">
         <v>547</v>
       </c>
@@ -21203,8 +21203,8 @@
       <c r="W13" s="102"/>
     </row>
     <row r="14" spans="1:23" ht="90">
-      <c r="A14" s="205"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="227"/>
+      <c r="B14" s="229"/>
       <c r="C14" s="96" t="s">
         <v>547</v>
       </c>
@@ -21258,8 +21258,8 @@
       <c r="W14" s="102"/>
     </row>
     <row r="15" spans="1:23" ht="90">
-      <c r="A15" s="205"/>
-      <c r="B15" s="207"/>
+      <c r="A15" s="227"/>
+      <c r="B15" s="229"/>
       <c r="C15" s="96" t="s">
         <v>547</v>
       </c>
@@ -21315,8 +21315,8 @@
       <c r="W15" s="102"/>
     </row>
     <row r="16" spans="1:23" ht="90">
-      <c r="A16" s="205"/>
-      <c r="B16" s="207"/>
+      <c r="A16" s="227"/>
+      <c r="B16" s="229"/>
       <c r="C16" s="96" t="s">
         <v>547</v>
       </c>
@@ -21370,8 +21370,8 @@
       <c r="W16" s="99"/>
     </row>
     <row r="17" spans="1:23" ht="90">
-      <c r="A17" s="205"/>
-      <c r="B17" s="208"/>
+      <c r="A17" s="227"/>
+      <c r="B17" s="230"/>
       <c r="C17" s="96" t="s">
         <v>547</v>
       </c>
@@ -21590,13 +21590,13 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="135">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="231" t="s">
         <v>529</v>
       </c>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="223" t="s">
         <v>781</v>
       </c>
-      <c r="C2" s="179" t="s">
+      <c r="C2" s="212" t="s">
         <v>786</v>
       </c>
       <c r="D2" s="26" t="s">
@@ -21655,9 +21655,9 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="90">
-      <c r="A3" s="209"/>
-      <c r="B3" s="201"/>
-      <c r="C3" s="181"/>
+      <c r="A3" s="231"/>
+      <c r="B3" s="223"/>
+      <c r="C3" s="214"/>
       <c r="D3" s="26" t="s">
         <v>481</v>
       </c>
@@ -21704,8 +21704,8 @@
       <c r="W3" s="64"/>
     </row>
     <row r="4" spans="1:23" ht="105">
-      <c r="A4" s="209"/>
-      <c r="B4" s="201"/>
+      <c r="A4" s="231"/>
+      <c r="B4" s="223"/>
       <c r="C4" s="35" t="s">
         <v>782</v>
       </c>
@@ -21765,8 +21765,8 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="105">
-      <c r="A5" s="209"/>
-      <c r="B5" s="201"/>
+      <c r="A5" s="231"/>
+      <c r="B5" s="223"/>
       <c r="C5" s="26" t="s">
         <v>783</v>
       </c>
@@ -21826,8 +21826,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="105">
-      <c r="A6" s="209"/>
-      <c r="B6" s="201"/>
+      <c r="A6" s="231"/>
+      <c r="B6" s="223"/>
       <c r="C6" s="26" t="s">
         <v>784</v>
       </c>
@@ -21887,8 +21887,8 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="105">
-      <c r="A7" s="209"/>
-      <c r="B7" s="201"/>
+      <c r="A7" s="231"/>
+      <c r="B7" s="223"/>
       <c r="C7" s="26" t="s">
         <v>785</v>
       </c>
@@ -22094,10 +22094,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="75">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="231" t="s">
         <v>530</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="206" t="s">
         <v>580</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -22153,8 +22153,8 @@
       <c r="W2" s="8"/>
     </row>
     <row r="3" spans="1:23" ht="270">
-      <c r="A3" s="209"/>
-      <c r="B3" s="186"/>
+      <c r="A3" s="231"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="24" t="s">
         <v>668</v>
       </c>
@@ -22208,8 +22208,8 @@
       <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" ht="75">
-      <c r="A4" s="209"/>
-      <c r="B4" s="186"/>
+      <c r="A4" s="231"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="35" t="s">
         <v>598</v>
       </c>
@@ -22265,9 +22265,9 @@
       <c r="W4" s="8"/>
     </row>
     <row r="5" spans="1:23" ht="90">
-      <c r="A5" s="209"/>
-      <c r="B5" s="186"/>
-      <c r="C5" s="210" t="s">
+      <c r="A5" s="231"/>
+      <c r="B5" s="207"/>
+      <c r="C5" s="218" t="s">
         <v>599</v>
       </c>
       <c r="D5" s="35" t="s">
@@ -22320,9 +22320,9 @@
       <c r="W5" s="20"/>
     </row>
     <row r="6" spans="1:23" ht="225">
-      <c r="A6" s="209"/>
-      <c r="B6" s="186"/>
-      <c r="C6" s="211"/>
+      <c r="A6" s="231"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="232"/>
       <c r="D6" s="35" t="s">
         <v>481</v>
       </c>
@@ -22373,9 +22373,9 @@
       <c r="W6" s="8"/>
     </row>
     <row r="7" spans="1:23" ht="90">
-      <c r="A7" s="209"/>
-      <c r="B7" s="186"/>
-      <c r="C7" s="211"/>
+      <c r="A7" s="231"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="232"/>
       <c r="D7" s="35" t="s">
         <v>481</v>
       </c>
@@ -22428,9 +22428,9 @@
       <c r="W7" s="8"/>
     </row>
     <row r="8" spans="1:23" ht="90">
-      <c r="A8" s="209"/>
-      <c r="B8" s="186"/>
-      <c r="C8" s="211"/>
+      <c r="A8" s="231"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="232"/>
       <c r="D8" s="35" t="s">
         <v>481</v>
       </c>
@@ -22481,9 +22481,9 @@
       <c r="W8" s="20"/>
     </row>
     <row r="9" spans="1:23" ht="90">
-      <c r="A9" s="209"/>
-      <c r="B9" s="187"/>
-      <c r="C9" s="212"/>
+      <c r="A9" s="231"/>
+      <c r="B9" s="208"/>
+      <c r="C9" s="219"/>
       <c r="D9" s="35" t="s">
         <v>481</v>
       </c>
@@ -22693,10 +22693,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="233" t="s">
         <v>531</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="206" t="s">
         <v>702</v>
       </c>
       <c r="C2" s="26" t="s">
@@ -22758,8 +22758,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" s="12" customFormat="1" ht="68.25" customHeight="1">
-      <c r="A3" s="214"/>
-      <c r="B3" s="186"/>
+      <c r="A3" s="234"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="23" t="s">
         <v>773</v>
       </c>
@@ -22819,9 +22819,9 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A4" s="214"/>
-      <c r="B4" s="186"/>
-      <c r="C4" s="203" t="s">
+      <c r="A4" s="234"/>
+      <c r="B4" s="207"/>
+      <c r="C4" s="225" t="s">
         <v>714</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -22880,9 +22880,9 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A5" s="214"/>
-      <c r="B5" s="186"/>
-      <c r="C5" s="203"/>
+      <c r="A5" s="234"/>
+      <c r="B5" s="207"/>
+      <c r="C5" s="225"/>
       <c r="D5" s="26" t="s">
         <v>481</v>
       </c>
@@ -22939,9 +22939,9 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A6" s="214"/>
-      <c r="B6" s="186"/>
-      <c r="C6" s="216" t="s">
+      <c r="A6" s="234"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="236" t="s">
         <v>703</v>
       </c>
       <c r="D6" s="26" t="s">
@@ -23000,9 +23000,9 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="214"/>
-      <c r="B7" s="186"/>
-      <c r="C7" s="216"/>
+      <c r="A7" s="234"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="236"/>
       <c r="D7" s="26" t="s">
         <v>481</v>
       </c>
@@ -23059,9 +23059,9 @@
       </c>
     </row>
     <row r="8" spans="1:23" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A8" s="214"/>
-      <c r="B8" s="186"/>
-      <c r="C8" s="216"/>
+      <c r="A8" s="234"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="236"/>
       <c r="D8" s="26" t="s">
         <v>481</v>
       </c>
@@ -23118,9 +23118,9 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A9" s="214"/>
-      <c r="B9" s="186"/>
-      <c r="C9" s="216"/>
+      <c r="A9" s="234"/>
+      <c r="B9" s="207"/>
+      <c r="C9" s="236"/>
       <c r="D9" s="26" t="s">
         <v>481</v>
       </c>
@@ -23177,9 +23177,9 @@
       </c>
     </row>
     <row r="10" spans="1:23" s="12" customFormat="1" ht="27" customHeight="1">
-      <c r="A10" s="214"/>
-      <c r="B10" s="186"/>
-      <c r="C10" s="216"/>
+      <c r="A10" s="234"/>
+      <c r="B10" s="207"/>
+      <c r="C10" s="236"/>
       <c r="D10" s="23" t="s">
         <v>481</v>
       </c>
@@ -23236,9 +23236,9 @@
       </c>
     </row>
     <row r="11" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A11" s="214"/>
-      <c r="B11" s="186"/>
-      <c r="C11" s="216"/>
+      <c r="A11" s="234"/>
+      <c r="B11" s="207"/>
+      <c r="C11" s="236"/>
       <c r="D11" s="26" t="s">
         <v>481</v>
       </c>
@@ -23295,9 +23295,9 @@
       </c>
     </row>
     <row r="12" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A12" s="214"/>
-      <c r="B12" s="186"/>
-      <c r="C12" s="216" t="s">
+      <c r="A12" s="234"/>
+      <c r="B12" s="207"/>
+      <c r="C12" s="236" t="s">
         <v>730</v>
       </c>
       <c r="D12" s="26" t="s">
@@ -23356,9 +23356,9 @@
       </c>
     </row>
     <row r="13" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A13" s="214"/>
-      <c r="B13" s="186"/>
-      <c r="C13" s="216"/>
+      <c r="A13" s="234"/>
+      <c r="B13" s="207"/>
+      <c r="C13" s="236"/>
       <c r="D13" s="26" t="s">
         <v>481</v>
       </c>
@@ -23415,9 +23415,9 @@
       </c>
     </row>
     <row r="14" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A14" s="214"/>
-      <c r="B14" s="186"/>
-      <c r="C14" s="216"/>
+      <c r="A14" s="234"/>
+      <c r="B14" s="207"/>
+      <c r="C14" s="236"/>
       <c r="D14" s="26" t="s">
         <v>481</v>
       </c>
@@ -23474,9 +23474,9 @@
       </c>
     </row>
     <row r="15" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A15" s="214"/>
-      <c r="B15" s="186"/>
-      <c r="C15" s="216"/>
+      <c r="A15" s="234"/>
+      <c r="B15" s="207"/>
+      <c r="C15" s="236"/>
       <c r="D15" s="26" t="s">
         <v>481</v>
       </c>
@@ -23533,9 +23533,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A16" s="214"/>
-      <c r="B16" s="186"/>
-      <c r="C16" s="216"/>
+      <c r="A16" s="234"/>
+      <c r="B16" s="207"/>
+      <c r="C16" s="236"/>
       <c r="D16" s="26" t="s">
         <v>481</v>
       </c>
@@ -23592,9 +23592,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" s="12" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A17" s="214"/>
-      <c r="B17" s="186"/>
-      <c r="C17" s="216"/>
+      <c r="A17" s="234"/>
+      <c r="B17" s="207"/>
+      <c r="C17" s="236"/>
       <c r="D17" s="26" t="s">
         <v>481</v>
       </c>
@@ -23651,9 +23651,9 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="24.75" customHeight="1">
-      <c r="A18" s="214"/>
-      <c r="B18" s="186"/>
-      <c r="C18" s="176" t="s">
+      <c r="A18" s="234"/>
+      <c r="B18" s="207"/>
+      <c r="C18" s="209" t="s">
         <v>766</v>
       </c>
       <c r="D18" s="26" t="s">
@@ -23712,9 +23712,9 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="26.25" customHeight="1">
-      <c r="A19" s="215"/>
-      <c r="B19" s="187"/>
-      <c r="C19" s="178"/>
+      <c r="A19" s="235"/>
+      <c r="B19" s="208"/>
+      <c r="C19" s="211"/>
       <c r="D19" s="26" t="s">
         <v>481</v>
       </c>

</xml_diff>